<commit_message>
Task 2c Step 5: Final changes
I updated the directories in Management.do, Analysis.do and the master file. I updated the Projectmap_AK91 and I deleted the old master.log and some old output results that I don't think it is useful to have here. Then I update the .gitignore to not have .tex and .log files.
</commit_message>
<xml_diff>
--- a/Projectmap_AK91.xlsx
+++ b/Projectmap_AK91.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xsalgi\Desktop\AK91\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xsalgi\Desktop\Task2\2b\AK91\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD442B6C-3981-441D-8A96-47B3F767C181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2266B2A6-0ED8-4CDC-AE0C-DA5956155CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{18D8AB28-A1D8-4E37-BEE3-285E2393BFE3}"/>
   </bookViews>
@@ -97,8 +97,8 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>359077</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>155726</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>170090</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -114,7 +114,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1998486" y="130024"/>
-          <a:ext cx="12443984" cy="4493381"/>
+          <a:ext cx="12443984" cy="6322030"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -150,13 +150,13 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>385081</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>59872</xdr:rowOff>
+      <xdr:rowOff>59871</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>368148</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>104322</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>158749</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -171,8 +171,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7120617" y="2599872"/>
-          <a:ext cx="6718602" cy="1790700"/>
+          <a:off x="7120617" y="2599871"/>
+          <a:ext cx="6718602" cy="3296557"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -605,203 +605,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Flowchart: Process 24">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F7D27B1-E0D7-3933-F984-6849441A636F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2901950" y="2216150"/>
-          <a:ext cx="1308100" cy="330200"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartProcess">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Table</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>IV_data.do</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="Flowchart: Process 25">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E838A12-4C73-4C0C-8DBA-166EEFF229AF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2901950" y="2603500"/>
-          <a:ext cx="1308100" cy="330200"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartProcess">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>TableV_data.do</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="Flowchart: Process 28">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A157C4F-CA00-46C6-BD1D-D5CDD6358B7B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2914650" y="3016250"/>
-          <a:ext cx="1308100" cy="330200"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartProcess">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>TableVI_data.do</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>336550</xdr:colOff>
       <xdr:row>15</xdr:row>
@@ -810,8 +613,8 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>11339</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -827,7 +630,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9521371" y="2732768"/>
-          <a:ext cx="1817915" cy="1518103"/>
+          <a:ext cx="1817915" cy="2834821"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -885,7 +688,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="49" name="TextBox 48">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{116B0F95-98B3-45E0-8338-66BE86793A01}"/>
@@ -940,80 +743,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="Flowchart: Process 50">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7271EED-34CF-484D-91AC-872486345C6D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5486400" y="2216150"/>
-          <a:ext cx="1308100" cy="330200"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartProcess">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>TableIV_analysis.do</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>908</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>147411</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>594179</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>45357</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1028,8 +767,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11612336" y="2721429"/>
-          <a:ext cx="1817914" cy="1523092"/>
+          <a:off x="11635015" y="2687411"/>
+          <a:ext cx="1817914" cy="2914196"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1087,7 +826,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="55" name="Flowchart: Process 54">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{382107E5-6155-4329-91AA-B836F1A48546}"/>
@@ -1128,7 +867,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>TableV_analysis.do</a:t>
+            <a:t>Analysis.do</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1137,70 +876,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="56" name="Flowchart: Process 55">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{508B88CD-4428-4254-9778-9BB85BA52077}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5461000" y="3003550"/>
-          <a:ext cx="1308100" cy="330200"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartProcess">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>TableVI_analysis.do</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>17</xdr:row>
@@ -1215,7 +890,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="58" name="Flowchart: Process 57">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A654A365-6B37-4525-85C7-9FD8EF1D51C7}"/>
@@ -1279,7 +954,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="60" name="Flowchart: Process 59">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDA4E82F-4344-4567-B851-59FFCA44D036}"/>
@@ -1343,7 +1018,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="62" name="Flowchart: Process 61">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B2AE6E9-1F42-4294-94B1-DB8FCA38E811}"/>
@@ -1407,7 +1082,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="64" name="TextBox 63">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BE40628-4A51-4C9A-96B8-7974BF62F0BA}"/>
@@ -1471,7 +1146,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="66" name="TextBox 65">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AC97775-3A1B-4F6F-8AC3-6DF249E26B4E}"/>
@@ -1535,7 +1210,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="68" name="TextBox 67">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17C1146B-2D6E-4174-AC7E-34ECB172D0A1}"/>
@@ -1599,7 +1274,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="70" name="TextBox 69">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81785003-8836-4D26-926D-185FC777A2AD}"/>
@@ -1649,226 +1324,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="72" name="Straight Arrow Connector 71">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93AFC91E-A8B9-505A-215B-55BF5054D3AF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="25" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2228850" y="2381250"/>
-          <a:ext cx="673100" cy="177800"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="74" name="Straight Arrow Connector 73">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F07F738C-82D4-DA43-F282-17FAB5690DE4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="26" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2228850" y="2584450"/>
-          <a:ext cx="673100" cy="184150"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="77" name="Straight Arrow Connector 76">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD19E0B4-E35F-4002-8C12-3FF14DA320B8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2241550" y="2609850"/>
-          <a:ext cx="660400" cy="603250"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>170090</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>236312</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="81" name="Straight Arrow Connector 80">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49F99949-9366-46FF-F4B4-75CDA4C221AD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="53" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="6076043" y="3254376"/>
-          <a:ext cx="1508126" cy="11338"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:colOff>555626</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
@@ -1880,21 +1337,22 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="82" name="Straight Arrow Connector 81">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B1C41E-DB58-4D06-B5E9-52F72B471CE4}"/>
+        <xdr:cNvPr id="74" name="Straight Arrow Connector 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F07F738C-82D4-DA43-F282-17FAB5690DE4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:endCxn id="57" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6063343" y="3605893"/>
-          <a:ext cx="1525815" cy="24039"/>
+          <a:off x="6066519" y="3605893"/>
+          <a:ext cx="1522639" cy="24039"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1923,9 +1381,120 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>542472</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>170090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>236312</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="Straight Arrow Connector 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49F99949-9366-46FF-F4B4-75CDA4C221AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="53" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6053365" y="3254376"/>
+          <a:ext cx="1530804" cy="345167"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>405039</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>147411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>453572</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="82" name="Straight Arrow Connector 81">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B1C41E-DB58-4D06-B5E9-52F72B471CE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4078968" y="3594554"/>
+          <a:ext cx="660854" cy="4989"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>566964</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>45358</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
@@ -1946,8 +1515,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6069693" y="3948793"/>
-          <a:ext cx="1504950" cy="8618"/>
+          <a:off x="6077857" y="3673929"/>
+          <a:ext cx="1496786" cy="283482"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1976,15 +1545,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>82550</xdr:colOff>
+      <xdr:colOff>68035</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>170089</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>56696</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2000,9 +1569,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6788150" y="2381250"/>
-          <a:ext cx="774700" cy="0"/>
+        <a:xfrm flipV="1">
+          <a:off x="11089821" y="3254375"/>
+          <a:ext cx="791936" cy="249464"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2084,15 +1653,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>102053</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>124733</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>260350</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>78468</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2109,8 +1678,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6781800" y="3149600"/>
-          <a:ext cx="793750" cy="25400"/>
+          <a:off x="11123839" y="3753304"/>
+          <a:ext cx="770618" cy="248557"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2152,7 +1721,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="91" name="Flowchart: Magnetic Disk 90">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93AF832A-12F2-4090-B5E0-F1C979EB3568}"/>
@@ -2268,7 +1837,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="93" name="Rectangle 92">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3574713A-CB62-4E52-8976-C02886B9E1B4}"/>
@@ -2475,7 +2044,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="53" name="Flowchart: Process 52">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFE3B4BA-5729-4F67-AEDD-241DA9BAF597}"/>
@@ -2539,7 +2108,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="57" name="Flowchart: Process 56">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{052AF387-9362-49FB-BD8C-D64FA83DBDEC}"/>
@@ -2603,7 +2172,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="59" name="Flowchart: Process 58">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D336707-1D8E-4B28-AD51-389A84EADB47}"/>
@@ -2667,7 +2236,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="61" name="TextBox 60">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02E54F23-1E51-4624-AD8A-5AF3AB2121C6}"/>
@@ -2720,13 +2289,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>325211</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>170089</xdr:rowOff>
+      <xdr:rowOff>170090</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>170090</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2738,14 +2307,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="53" idx="3"/>
-          <a:endCxn id="51" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8897711" y="3254375"/>
-          <a:ext cx="899432" cy="1"/>
+        <a:xfrm>
+          <a:off x="8897711" y="3254376"/>
+          <a:ext cx="899432" cy="260803"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2828,12 +2397,12 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>340179</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>45357</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>14968</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>45358</xdr:rowOff>
     </xdr:to>
@@ -2850,8 +2419,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8912679" y="3968750"/>
-          <a:ext cx="899432" cy="1"/>
+          <a:off x="8912679" y="3787321"/>
+          <a:ext cx="884464" cy="181430"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2893,7 +2462,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="86" name="TextBox 85">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8F875BC-2451-3626-4A77-856423F99230}"/>
@@ -2944,6 +2513,540 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>453572</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>170090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>542472</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>134711</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Flowchart: Process 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD5786B6-87E0-4E92-AD43-CA93FB4409A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4739822" y="3435804"/>
+          <a:ext cx="1313543" cy="327478"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Management.do</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>260803</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>349703</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>146049</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Flowchart: Process 27">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2788C98-9C2E-4B43-A1ED-2FC12E82AEEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11894910" y="4286250"/>
+          <a:ext cx="1313543" cy="327478"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>TableIV_p.tex</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>272144</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>361044</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>78014</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Flowchart: Process 29">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67452C24-F790-4223-9485-244ED7D426AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11906251" y="4762500"/>
+          <a:ext cx="1313543" cy="327478"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>TableV_p.tex</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>272144</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>361044</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Flowchart: Process 30">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D997A160-9F59-493B-9F45-82708B918E57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11906251" y="5193393"/>
+          <a:ext cx="1313543" cy="327478"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>TableVI_p.tex</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>578304</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>249464</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>147411</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Arrow Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0952BE7-43D2-420D-80B3-633D7273A349}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10987768" y="3810000"/>
+          <a:ext cx="895803" cy="623661"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>204107</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>34017</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>260804</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Arrow Connector 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CC3F2DB-D9BD-4050-A366-7177600FD192}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10613571" y="3844017"/>
+          <a:ext cx="1281340" cy="1099912"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>544285</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>181428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>272144</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>163739</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Arrow Connector 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0580745F-DFEF-4040-8069-BBB04253A0DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="31" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10341428" y="3809999"/>
+          <a:ext cx="1564823" cy="1547133"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>34018</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>56697</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>125640</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>21318</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Flowchart: Process 42">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBAB710F-C20B-4039-AC31-8022515378F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9831161" y="4887233"/>
+          <a:ext cx="1316265" cy="327478"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>program_stata.do</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>408214</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>408215</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>11339</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Arrow Connector 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87403559-49F8-4EF8-AFB6-5E2B3776B432}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10205357" y="3787321"/>
+          <a:ext cx="1" cy="1054554"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3248,8 +3351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450FFCD6-3198-412C-A79D-7BC785AC8D22}">
   <dimension ref="A22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="AB27" sqref="AB27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>